<commit_message>
add Katarzyna Burda, Mateusz Konczal
</commit_message>
<xml_diff>
--- a/mutation_rate_literature_updating3.xlsx
+++ b/mutation_rate_literature_updating3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ywang120\Desktop\mutation_literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A070218D-61DB-4DF3-84DF-C617C67EDA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD49BBB1-319F-4C23-AB3A-04E3FB3D12D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27900" yWindow="-2556" windowWidth="22704" windowHeight="14592" xr2:uid="{09A42BD9-4349-4213-8D0A-A379C870C482}"/>
+    <workbookView xWindow="23352" yWindow="-3960" windowWidth="23040" windowHeight="12264" xr2:uid="{09A42BD9-4349-4213-8D0A-A379C870C482}"/>
   </bookViews>
   <sheets>
     <sheet name="raw" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8783" uniqueCount="2269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8799" uniqueCount="2276">
   <si>
     <t>PID</t>
   </si>
@@ -6849,6 +6849,27 @@
   </si>
   <si>
     <t>https://www.biorxiv.org/content/10.1101/2023.06.28.546961v1</t>
+  </si>
+  <si>
+    <t>2023006_01</t>
+  </si>
+  <si>
+    <t>Illumina NovaSeq 6000</t>
+  </si>
+  <si>
+    <t>1.92e-9</t>
+  </si>
+  <si>
+    <t>3.88e-9</t>
+  </si>
+  <si>
+    <t>47X</t>
+  </si>
+  <si>
+    <t>Burda, K., &amp; Konczal, M. (2023). Validation of machine learning approach for direct mutation rate estimation. Molecular Ecology Resources, 00, 1– 15. https://doi.org/10.1111/1755-0998.13841</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/full/10.1111/1755-0998.13841</t>
   </si>
 </sst>
 </file>
@@ -7240,12 +7261,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{318201D5-CE15-42FE-AD6F-C948F9B6134A}">
-  <dimension ref="A1:AC501"/>
+  <dimension ref="A1:AC502"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A479" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="M504" sqref="M504"/>
+      <selection pane="bottomLeft" activeCell="K495" sqref="K495"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40383,6 +40404,71 @@
       </c>
       <c r="AC501" s="2" t="s">
         <v>2268</v>
+      </c>
+    </row>
+    <row r="502" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A502">
+        <v>2023006</v>
+      </c>
+      <c r="B502">
+        <v>2023</v>
+      </c>
+      <c r="C502" t="s">
+        <v>188</v>
+      </c>
+      <c r="D502" t="s">
+        <v>188</v>
+      </c>
+      <c r="E502" s="5" t="s">
+        <v>2012</v>
+      </c>
+      <c r="F502" t="s">
+        <v>2013</v>
+      </c>
+      <c r="H502" t="s">
+        <v>2269</v>
+      </c>
+      <c r="I502" t="s">
+        <v>2020</v>
+      </c>
+      <c r="J502" t="s">
+        <v>30</v>
+      </c>
+      <c r="K502" t="s">
+        <v>31</v>
+      </c>
+      <c r="L502" s="1" t="s">
+        <v>1194</v>
+      </c>
+      <c r="M502" s="1" t="s">
+        <v>2271</v>
+      </c>
+      <c r="N502" s="1" t="s">
+        <v>2272</v>
+      </c>
+      <c r="R502" s="6">
+        <v>21</v>
+      </c>
+      <c r="T502" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="U502">
+        <v>24</v>
+      </c>
+      <c r="V502">
+        <v>1</v>
+      </c>
+      <c r="W502" s="1" t="s">
+        <v>2270</v>
+      </c>
+      <c r="Y502" t="s">
+        <v>2273</v>
+      </c>
+      <c r="AA502" t="s">
+        <v>2274</v>
+      </c>
+      <c r="AC502" s="2" t="s">
+        <v>2275</v>
       </c>
     </row>
   </sheetData>
@@ -40811,6 +40897,7 @@
     <hyperlink ref="AC499" r:id="rId421" xr:uid="{68B472BE-11B8-4E2C-9783-AAC12870590E}"/>
     <hyperlink ref="AC500" r:id="rId422" xr:uid="{B9A7A64F-F3A3-4D8D-A7A7-F9435A0FDD30}"/>
     <hyperlink ref="AC501" r:id="rId423" xr:uid="{F1186383-B365-495B-9DB1-CF21BCAEFE16}"/>
+    <hyperlink ref="AC502" r:id="rId424" xr:uid="{9CFB9B5E-10DE-4AB1-B1B8-492CF07EAF2B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add 'Liang. X, Commun Biol'
</commit_message>
<xml_diff>
--- a/mutation_rate_literature_updating3.xlsx
+++ b/mutation_rate_literature_updating3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yigua\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD260BAB-529A-4E6F-8999-721EB0CB2003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DAEC8F8-1FD2-4FE0-87D5-B415D0D72770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9950" yWindow="3420" windowWidth="23870" windowHeight="16130" xr2:uid="{09A42BD9-4349-4213-8D0A-A379C870C482}"/>
+    <workbookView xWindow="16380" yWindow="4160" windowWidth="18040" windowHeight="15370" xr2:uid="{09A42BD9-4349-4213-8D0A-A379C870C482}"/>
   </bookViews>
   <sheets>
     <sheet name="raw" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8845" uniqueCount="2302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8862" uniqueCount="2317">
   <si>
     <t>PID</t>
   </si>
@@ -6961,6 +6961,66 @@
   </si>
   <si>
     <t>https://www.sciencedirect.com/science/article/pii/S2211926424003060</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>zebra finches</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taeniopygia guttata</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Australia</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024003_01</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>sexual</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>snp</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.36e-9</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.32e-9</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.60e-9</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>PO</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Illumina TruSeq</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>49X</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Liang, X., Yang, S., Wang, D. et al. Characterization and distribution of de novo mutations in the zebra finch. Commun Biol 7, 1243 (2024). https://doi.org/10.1038/s42003-024-06945-5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.nature.com/articles/s42003-024-06945-5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>birds</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -7368,12 +7428,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{318201D5-CE15-42FE-AD6F-C948F9B6134A}">
-  <dimension ref="A1:AC505"/>
+  <dimension ref="A1:AC506"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A482" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A473" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="V509" sqref="V509"/>
+      <selection pane="bottomLeft" activeCell="X495" sqref="X495"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -40766,6 +40826,71 @@
       </c>
       <c r="AC505" s="1" t="s">
         <v>2301</v>
+      </c>
+    </row>
+    <row r="506" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A506">
+        <v>2024003</v>
+      </c>
+      <c r="B506">
+        <v>2024</v>
+      </c>
+      <c r="C506" t="s">
+        <v>2316</v>
+      </c>
+      <c r="D506" t="s">
+        <v>2316</v>
+      </c>
+      <c r="E506" s="7" t="s">
+        <v>2302</v>
+      </c>
+      <c r="F506" t="s">
+        <v>2303</v>
+      </c>
+      <c r="G506" t="s">
+        <v>2304</v>
+      </c>
+      <c r="H506" t="s">
+        <v>2305</v>
+      </c>
+      <c r="I506" t="s">
+        <v>2306</v>
+      </c>
+      <c r="J506" t="s">
+        <v>2307</v>
+      </c>
+      <c r="K506" t="s">
+        <v>31</v>
+      </c>
+      <c r="L506" s="4" t="s">
+        <v>2308</v>
+      </c>
+      <c r="M506" s="4" t="s">
+        <v>2309</v>
+      </c>
+      <c r="N506" s="4" t="s">
+        <v>2310</v>
+      </c>
+      <c r="R506" s="8">
+        <v>105</v>
+      </c>
+      <c r="T506" s="4" t="s">
+        <v>2311</v>
+      </c>
+      <c r="U506">
+        <v>4</v>
+      </c>
+      <c r="W506" s="4" t="s">
+        <v>2312</v>
+      </c>
+      <c r="Y506" t="s">
+        <v>2313</v>
+      </c>
+      <c r="AA506" t="s">
+        <v>2314</v>
+      </c>
+      <c r="AC506" s="1" t="s">
+        <v>2315</v>
       </c>
     </row>
   </sheetData>
@@ -41199,6 +41324,7 @@
     <hyperlink ref="AC503" r:id="rId425" xr:uid="{B9B868B2-A9CF-415F-B2C8-A71B021703C3}"/>
     <hyperlink ref="AC504" r:id="rId426" xr:uid="{187E2094-C54D-4707-9DAC-C00BC73602BA}"/>
     <hyperlink ref="AC505" r:id="rId427" xr:uid="{AA3DE5F5-8CEA-4EDE-ACF1-28C535A726DD}"/>
+    <hyperlink ref="AC506" r:id="rId428" xr:uid="{2FD49CDB-3C46-4CF7-864E-4E156705A06E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add "Lisa Mettrop et al. 2025, GBE"
</commit_message>
<xml_diff>
--- a/mutation_rate_literature_updating3.xlsx
+++ b/mutation_rate_literature_updating3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ywang120\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D57E35C-8A53-4350-99AF-E5A0E5FDD9B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68620EC-093B-4469-A85A-3BF7DB9672E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4880" yWindow="6070" windowWidth="25610" windowHeight="11310" xr2:uid="{09A42BD9-4349-4213-8D0A-A379C870C482}"/>
+    <workbookView xWindow="7210" yWindow="2680" windowWidth="28800" windowHeight="15540" xr2:uid="{09A42BD9-4349-4213-8D0A-A379C870C482}"/>
   </bookViews>
   <sheets>
     <sheet name="raw" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">gs_gt!$A$1:$E$129</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">raw!$A$1:$AC$500</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">raw!$A$1:$AC$511</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8918" uniqueCount="2326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8976" uniqueCount="2336">
   <si>
     <t>PID</t>
   </si>
@@ -7049,6 +7049,36 @@
   </si>
   <si>
     <t>4.22e-9</t>
+  </si>
+  <si>
+    <t>Prasinoderma coloniale</t>
+  </si>
+  <si>
+    <t>211..641</t>
+  </si>
+  <si>
+    <t>2025001_01</t>
+  </si>
+  <si>
+    <t>1.18e-10</t>
+  </si>
+  <si>
+    <t>2.19e-10</t>
+  </si>
+  <si>
+    <t>3.40e-11</t>
+  </si>
+  <si>
+    <t>6.45e-11</t>
+  </si>
+  <si>
+    <t>Illumina NovaSeq 4000</t>
+  </si>
+  <si>
+    <t>Mettrop, L., Lipzen, A., Vandecasteele, C., Eché, C., Labécot, A., Barry, K., ... &amp; Krasovec, M. (2025). Low Mutation Rate and Atypical Mutation Spectrum in Prasinoderma coloniale: Insights From an Early Diverging Green Lineage. Genome Biology and Evolution, 17(3), evaf026.</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/gbe/article/17/3/evaf026/8058679?login=true</t>
   </si>
 </sst>
 </file>
@@ -7455,12 +7485,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{318201D5-CE15-42FE-AD6F-C948F9B6134A}">
-  <dimension ref="A1:AC510"/>
+  <dimension ref="A1:AC514"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A488" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A480" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="M508" sqref="M508"/>
+      <selection pane="bottomLeft" activeCell="A515" sqref="A515"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -41144,8 +41174,238 @@
         <v>2322</v>
       </c>
     </row>
+    <row r="511" spans="1:29">
+      <c r="A511">
+        <v>2025001</v>
+      </c>
+      <c r="B511">
+        <v>2025</v>
+      </c>
+      <c r="C511" t="s">
+        <v>37</v>
+      </c>
+      <c r="D511" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E511" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="F511" t="s">
+        <v>2326</v>
+      </c>
+      <c r="H511" t="s">
+        <v>2328</v>
+      </c>
+      <c r="I511" t="s">
+        <v>2019</v>
+      </c>
+      <c r="J511" t="s">
+        <v>30</v>
+      </c>
+      <c r="K511" t="s">
+        <v>31</v>
+      </c>
+      <c r="L511" s="4" t="s">
+        <v>1704</v>
+      </c>
+      <c r="M511" s="4" t="s">
+        <v>2329</v>
+      </c>
+      <c r="N511" s="4" t="s">
+        <v>2330</v>
+      </c>
+      <c r="R511" s="8">
+        <v>43</v>
+      </c>
+      <c r="T511" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="U511">
+        <v>25</v>
+      </c>
+      <c r="V511" t="s">
+        <v>2327</v>
+      </c>
+      <c r="W511" s="4" t="s">
+        <v>2333</v>
+      </c>
+      <c r="AA511" t="s">
+        <v>2334</v>
+      </c>
+      <c r="AC511" s="1" t="s">
+        <v>2335</v>
+      </c>
+    </row>
+    <row r="512" spans="1:29">
+      <c r="A512">
+        <v>2025001</v>
+      </c>
+      <c r="B512">
+        <v>2025</v>
+      </c>
+      <c r="C512" t="s">
+        <v>37</v>
+      </c>
+      <c r="D512" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E512" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="F512" t="s">
+        <v>2326</v>
+      </c>
+      <c r="H512" t="s">
+        <v>2328</v>
+      </c>
+      <c r="I512" t="s">
+        <v>2019</v>
+      </c>
+      <c r="J512" t="s">
+        <v>59</v>
+      </c>
+      <c r="K512" t="s">
+        <v>31</v>
+      </c>
+      <c r="L512" s="4" t="s">
+        <v>2331</v>
+      </c>
+      <c r="M512" s="4" t="s">
+        <v>1084</v>
+      </c>
+      <c r="N512" s="4" t="s">
+        <v>2332</v>
+      </c>
+      <c r="R512" s="8">
+        <v>9</v>
+      </c>
+      <c r="T512" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="U512">
+        <v>25</v>
+      </c>
+      <c r="V512" t="s">
+        <v>2327</v>
+      </c>
+      <c r="W512" s="4" t="s">
+        <v>2333</v>
+      </c>
+      <c r="AA512" t="s">
+        <v>2334</v>
+      </c>
+      <c r="AC512" s="1" t="s">
+        <v>2335</v>
+      </c>
+    </row>
+    <row r="513" spans="1:29">
+      <c r="A513">
+        <v>2025001</v>
+      </c>
+      <c r="B513">
+        <v>2025</v>
+      </c>
+      <c r="C513" t="s">
+        <v>37</v>
+      </c>
+      <c r="D513" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E513" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="F513" t="s">
+        <v>2326</v>
+      </c>
+      <c r="H513" t="s">
+        <v>2328</v>
+      </c>
+      <c r="I513" t="s">
+        <v>2019</v>
+      </c>
+      <c r="J513" t="s">
+        <v>61</v>
+      </c>
+      <c r="K513" t="s">
+        <v>31</v>
+      </c>
+      <c r="R513" s="8">
+        <v>2</v>
+      </c>
+      <c r="T513" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="U513">
+        <v>25</v>
+      </c>
+      <c r="V513" t="s">
+        <v>2327</v>
+      </c>
+      <c r="W513" s="4" t="s">
+        <v>2333</v>
+      </c>
+      <c r="AA513" t="s">
+        <v>2334</v>
+      </c>
+      <c r="AC513" s="1" t="s">
+        <v>2335</v>
+      </c>
+    </row>
+    <row r="514" spans="1:29">
+      <c r="A514">
+        <v>2025001</v>
+      </c>
+      <c r="B514">
+        <v>2025</v>
+      </c>
+      <c r="C514" t="s">
+        <v>37</v>
+      </c>
+      <c r="D514" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E514" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="F514" t="s">
+        <v>2326</v>
+      </c>
+      <c r="H514" t="s">
+        <v>2328</v>
+      </c>
+      <c r="I514" t="s">
+        <v>2019</v>
+      </c>
+      <c r="J514" t="s">
+        <v>60</v>
+      </c>
+      <c r="K514" t="s">
+        <v>31</v>
+      </c>
+      <c r="R514" s="8">
+        <v>7</v>
+      </c>
+      <c r="T514" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="U514">
+        <v>25</v>
+      </c>
+      <c r="V514" t="s">
+        <v>2327</v>
+      </c>
+      <c r="W514" s="4" t="s">
+        <v>2333</v>
+      </c>
+      <c r="AA514" t="s">
+        <v>2334</v>
+      </c>
+      <c r="AC514" s="1" t="s">
+        <v>2335</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AC500" xr:uid="{318201D5-CE15-42FE-AD6F-C948F9B6134A}"/>
+  <autoFilter ref="A1:AC511" xr:uid="{318201D5-CE15-42FE-AD6F-C948F9B6134A}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="AC12" r:id="rId1" xr:uid="{45A84390-3CC1-4266-9E84-77D0AEF55CBF}"/>
@@ -41580,6 +41840,10 @@
     <hyperlink ref="AC508" r:id="rId430" xr:uid="{B342DF92-87E4-4AA1-A24D-F74CFAC50A3D}"/>
     <hyperlink ref="AC509" r:id="rId431" xr:uid="{2796B3A9-3F3F-41A9-9C15-0A5784543185}"/>
     <hyperlink ref="AC510" r:id="rId432" xr:uid="{E9854539-678D-4DFC-B47B-DD11548DDAC0}"/>
+    <hyperlink ref="AC511" r:id="rId433" xr:uid="{5BBD3740-3E30-4BFB-AB82-6FA397A3E459}"/>
+    <hyperlink ref="AC512" r:id="rId434" xr:uid="{F037E0F8-3B23-45FE-8165-8B739B62E80A}"/>
+    <hyperlink ref="AC513" r:id="rId435" xr:uid="{314D50C6-FC2D-4439-A94D-6441CC03E2A8}"/>
+    <hyperlink ref="AC514" r:id="rId436" xr:uid="{C5EDDC40-D5C8-451D-9C79-15EF548A430B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>